<commit_message>
Updated ZIP and form definition files
</commit_message>
<xml_diff>
--- a/extras/test-form/Counter with timer.xlsx
+++ b/extras/test-form/Counter with timer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/counter-with-timer/extras/test-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF266236-04EE-B840-B60B-76D5E6E008FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F481AA5-08BC-AD4A-9283-56CBAB7B9E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2645,7 +2645,7 @@
     <t>counter_with_timer</t>
   </si>
   <si>
-    <t>custom-countertimer(A=10000, B='cs')</t>
+    <t>custom-counterwithtimer(duration=10, time-unit='cs')</t>
   </si>
 </sst>
 </file>
@@ -4803,7 +4803,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5432,7 +5432,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2002282030</v>
+        <v>2004091938</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>
@@ -6024,7 +6024,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" s="45" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" s="45" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="43" t="s">
         <v>93</v>
       </c>

</xml_diff>